<commit_message>
Update .gitignore to include _patch.py and add new generated xlsx files for XACML outputs
</commit_message>
<xml_diff>
--- a/_gen_outputs/xacml/xacml2_1.xml.xlsx
+++ b/_gen_outputs/xacml/xacml2_1.xml.xlsx
@@ -453,22 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>&lt;PolicySet xmlns="urn:oasis:names:tc:xacml:2.0:policy:schema:os" PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist"&gt;
-    &lt;Target/&gt;
-    &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.2"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;paper_review_content_rating_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.2.0"&gt;
-            &lt;Target/&gt;
-            &lt;Policy PolicyId="RPSlist.2.0.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.2.0.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                 &lt;Target&gt;
                     &lt;Subjects&gt;
                         &lt;Subject&gt;
@@ -504,10 +489,10 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S), has_role(S, role), has_attribute(S, isEq-subjUserId-resUserId, value).",
-    "datalog_objects": "Resource(R), has_resource_id(R, resource_id).",
-    "datalog_relationships": "is_paper_review_content_rating_rc(R) :- Resource(R), has_resource_id(R, 'paper_review_content_rating_rc').",
-    "datalog_actions": "deny_access(S, R) :- Subject(S), Resource(R), has_role(S, 'admin'), has_attribute(S, isEq-subjUserId-resUserId, 'false'), is_paper_review_content_rating_rc(R)."
+    "datalog_subjects": "Subject(S).",
+    "datalog_objects": "Resource(R).",
+    "datalog_relationships": "has_role(S, admin) :- Subject(S).\nisEq_subjUserId_resUserId(S, false) :- Subject(S).",
+    "datalog_actions": "deny_access(S, R) :- Subject(S), Resource(R), has_role(S, admin), isEq_subjUserId_resUserId(S, false)."
 }</t>
         </is>
       </c>
@@ -515,9 +500,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.2.0.4"&gt;
-                &lt;Target/&gt;
-                &lt;Policy PolicyId="RPSlist.2.0.4.3" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.2.0.4.3" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                     &lt;Target/&gt;
                     &lt;Rule Effect="Deny" RuleId="RPSlist.2.0.4.3.r.1"&gt;
                         &lt;Target/&gt;
@@ -551,22 +534,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.3"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;ismeetingflag_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.3.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.3.0.3"&gt;
-                &lt;Target/&gt;
-                &lt;Policy PolicyId="RPSlist.3.0.3.3" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.3.0.3.3" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                     &lt;Target&gt;
                         &lt;Subjects&gt;
                             &lt;Subject&gt;
@@ -606,10 +574,10 @@
       <c r="C4" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S) :- role(S, 'admin').",
-    "datalog_objects": "Resource(R) :- resource_id(R, 'ismeetingflag_rc').",
-    "datalog_relationships": "",
-    "datalog_actions": "can_access(S, R, 'write') :- Subject(S), Resource(R), role(S, 'admin'), resource_id(R, 'ismeetingflag_rc')."
+    "datalog_subjects": "User(U).",
+    "datalog_objects": "Resource(R).",
+    "datalog_relationships": "has_role(U, 'admin') :- User(U).",
+    "datalog_actions": "can_access(U, R, 'write') :- User(U), Resource(R), has_role(U, 'admin')."
 }</t>
         </is>
       </c>
@@ -617,24 +585,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.4"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;ismeetingflag_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.4.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.4.0.3"&gt;
-                &lt;Target/&gt;
-                &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.4.0.3.4"&gt;
-                    &lt;Target/&gt;
-                    &lt;Policy PolicyId="RPSlist.4.0.3.4.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.4.0.3.4.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                         &lt;Target&gt;
                             &lt;Subjects&gt;
 &lt;Subject&gt;
@@ -678,10 +629,10 @@
       <c r="C5" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "User(U), Role(U, R), IsMeeting(U, M).",
-    "datalog_objects": "Resource(Res).",
-    "datalog_relationships": "is_meeting_flag_rc(Res) :- Resource(Res).",
-    "datalog_actions": "can_read(U, Res) :- User(U), Resource(Res), Role(U, \"admin\"), IsMeeting(U, \"false\"), is_meeting_flag_rc(Res)."
+    "datalog_subjects": "User(U).",
+    "datalog_objects": "Resource(R).",
+    "datalog_relationships": "has_role(U, \"admin\") :- User(U).\nnot_in_meeting(U) :- User(U).",
+    "datalog_actions": "can_access(U, R, \"read\") :- User(U), Resource(R), has_role(U, \"admin\"), not_in_meeting(U)."
 }</t>
         </is>
       </c>
@@ -689,22 +640,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.5"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;paper_review_content_rating_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.5.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.5.0.0"&gt;
-                &lt;Target/&gt;
-                &lt;Policy PolicyId="RPSlist.5.0.0.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.5.0.0.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                     &lt;Target&gt;
                         &lt;Subjects&gt;
                             &lt;Subject&gt;
@@ -750,10 +686,10 @@
       <c r="C6" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S), role(S, R).",
-    "datalog_objects": "Resource(Res), resource_id(Res, ID).",
-    "datalog_relationships": "",
-    "datalog_actions": "can_access(S, Res, Action) :- Subject(S), Resource(Res), Action(Action), role(S, 'admin'), resource_id(Res, 'paper_review_content_rating_rc'), Action = 'write'."
+    "datalog_subjects": "Subject(S).",
+    "datalog_objects": "",
+    "datalog_relationships": "has_role(S, \"admin\") :- Subject(S).",
+    "datalog_actions": "can_perform(S, \"write\") :- Subject(S), has_role(S, \"admin\")."
 }</t>
         </is>
       </c>
@@ -803,8 +739,8 @@
           <t>{
     "datalog_subjects": "User(U).",
     "datalog_objects": "Resource(R).",
-    "datalog_relationships": "has_role(U, 'admin') :- User(U).",
-    "datalog_actions": "can_access(U, R, 'write') :- User(U), Resource(R), has_role(U, 'admin')."
+    "datalog_relationships": "has_role(U, \"admin\") :- User(U).",
+    "datalog_actions": "can_write(U, R) :- User(U), Resource(R), has_role(U, \"admin\")."
 }</t>
         </is>
       </c>
@@ -812,24 +748,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.6"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;paper_review_content_rating_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.6.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.6.0.3"&gt;
-                &lt;Target/&gt;
-                &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.6.0.3.4"&gt;
-                    &lt;Target/&gt;
-                    &lt;Policy PolicyId="RPSlist.6.0.3.4.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.6.0.3.4.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                         &lt;Target&gt;
                             &lt;Subjects&gt;
 &lt;Subject&gt;
@@ -875,10 +794,10 @@
       <c r="C8" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "User(U), Role(R).",
-    "datalog_objects": "Resource(Res).",
-    "datalog_relationships": "has_role(U, R) :- User(U), Role(R).",
-    "datalog_actions": "can_access(U, Res, Action) :- User(U), Resource(Res), Action(Action), has_role(U, 'admin'), Res = 'paper_review_content_rating_rc', (Action = 'read'; Action = 'write')."
+    "datalog_subjects": "Subject(S), role(S, R).",
+    "datalog_objects": "Object(O).",
+    "datalog_relationships": "",
+    "datalog_actions": "can_access(S, O, Action) :- Subject(S), Object(O), role(S, \"admin\"), (Action = \"read\"; Action = \"write\")."
 }</t>
         </is>
       </c>
@@ -932,8 +851,8 @@
           <t>{
     "datalog_subjects": "User(U).",
     "datalog_objects": "Resource(R).",
-    "datalog_relationships": "has_role(U, \"admin\") :- User(U).\nnot_in_meeting(U) :- User(U).",
-    "datalog_actions": "can_read(U, R) :- User(U), Resource(R), has_role(U, \"admin\"), not_in_meeting(U)."
+    "datalog_relationships": "has_role(U, \"admin\") :- User(U). has_isMeeting(U, \"false\") :- User(U).",
+    "datalog_actions": "can_access(U, R, \"read\") :- User(U), Resource(R), has_role(U, \"admin\"), has_isMeeting(U, \"false\")."
 }</t>
         </is>
       </c>
@@ -941,20 +860,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.9"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;ismeetingflag_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.9.0"&gt;
-            &lt;Target/&gt;
-            &lt;Policy PolicyId="RPSlist.9.0.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.9.0.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                 &lt;Target&gt;
                     &lt;Subjects&gt;
                         &lt;Subject&gt;
@@ -994,10 +900,10 @@
       <c r="C10" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S).",
-    "datalog_objects": "Resource(R).",
-    "datalog_relationships": "has_role(S, 'admin') :- Subject(S).",
-    "datalog_actions": "can_access(S, R, 'write') :- Subject(S), Resource(R), has_role(S, 'admin'), resource_id(R, 'ismeetingflag_rc')."
+    "datalog_subjects": "Subject(S), Role(R).",
+    "datalog_objects": "Resource(Res).",
+    "datalog_relationships": "has_role(S, R) :- Subject(S), Role(R).",
+    "datalog_actions": "can_access(S, Res, write) :- Subject(S), Resource(Res), has_role(S, admin)."
 }</t>
         </is>
       </c>
@@ -1005,9 +911,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.9.0.3"&gt;
-                &lt;Target/&gt;
-                &lt;Policy PolicyId="RPSlist.9.0.3.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.9.0.3.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                     &lt;Target&gt;
                         &lt;Subjects&gt;
                             &lt;Subject&gt;
@@ -1053,8 +957,8 @@
           <t>{
     "datalog_subjects": "Subject(S).",
     "datalog_objects": "Resource(R).",
-    "datalog_relationships": "",
-    "datalog_actions": "can_access(S, R, read) :- Subject(S), Resource(R), role(S, false), isMeeting(S, admin)."
+    "datalog_relationships": "has_role(S, \"false\") :- Subject(S).\nhas_isMeeting(S, \"admin\") :- Subject(S).",
+    "datalog_actions": "can_access(S, R, \"read\") :- Subject(S), Resource(R), has_role(S, \"false\"), has_isMeeting(S, \"admin\")."
 }</t>
         </is>
       </c>
@@ -1062,22 +966,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.10"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;paper_review_content_rating_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.10.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.10.0.0"&gt;
-                &lt;Target/&gt;
-                &lt;Policy PolicyId="RPSlist.10.0.0.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.10.0.0.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                     &lt;Target&gt;
                         &lt;Subjects&gt;
                             &lt;Subject&gt;
@@ -1123,8 +1012,8 @@
           <t>{
     "datalog_subjects": "Subject(S).",
     "datalog_objects": "Resource(R).",
-    "datalog_relationships": "has_role(S, 'admin') :- Subject(S).\nis_not_eq_subjUserId_resUserId(S) :- Subject(S).",
-    "datalog_actions": "can_access(S, R, 'read') :- Subject(S), Resource(R), has_role(S, 'admin'), is_not_eq_subjUserId_resUserId(S)."
+    "datalog_relationships": "has_role(S, 'admin') :- Subject(S).\nisEq_subjUserId_resUserId(S, 'false') :- Subject(S).",
+    "datalog_actions": "can_access(S, R, 'read') :- Subject(S), Resource(R), has_role(S, 'admin'), isEq_subjUserId_resUserId(S, 'false')."
 }</t>
         </is>
       </c>
@@ -1132,22 +1021,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.13"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;paper_review_content_rating_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.13.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.13.0.1"&gt;
-                &lt;Target/&gt;
-                &lt;Policy PolicyId="RPSlist.13.0.1.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.13.0.1.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                     &lt;Target&gt;
                         &lt;Subjects&gt;
                             &lt;Subject&gt;
@@ -1195,10 +1069,10 @@
       <c r="C13" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S), role(S, R).",
-    "datalog_objects": "Resource(Res), resource_id(Res, ResID), isEq_meetingPaper_resId(Res, ResID2).",
+    "datalog_subjects": "Admin(S) :- Subject(S), role(S, \"admin\").",
+    "datalog_objects": "Resource(R) :- Resource(R), isEq-meetingPaper-resId(R, \"paper_review_content_rating_rc\").",
     "datalog_relationships": "",
-    "datalog_actions": "can_access(S, Res, Action) :- Subject(S), Resource(Res), role(S, 'admin'), resource_id(Res, 'paper_review_content_rating_rc'), isEq_meetingPaper_resId(Res, 'paper_review_content_rating_rc'), Action = 'read'."
+    "datalog_actions": "can_read(S, R) :- Admin(S), Resource(R), action(S, \"read\")."
 }</t>
         </is>
       </c>
@@ -1206,20 +1080,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.14"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;ismeetingflag_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.14.0"&gt;
-            &lt;Target/&gt;
-            &lt;Policy PolicyId="RPSlist.14.0.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.14.0.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                 &lt;Target&gt;
                     &lt;Subjects&gt;
                         &lt;Subject&gt;
@@ -1271,10 +1132,10 @@
       <c r="C14" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S), role(S, R).",
-    "datalog_objects": "Resource(RES).",
-    "datalog_relationships": "resource_is_meeting_flag(RES) :- Resource(RES), RES = \"ismeetingflag_rc\".",
-    "datalog_actions": "can_access(S, RES, Action) :- Subject(S), Resource(RES), role(S, \"admin\"), resource_is_meeting_flag(RES), (Action = \"read\"; Action = \"write\")."
+    "datalog_subjects": "Subject(S).",
+    "datalog_objects": "Object(O).",
+    "datalog_relationships": "has_role(S, 'admin') :- Subject(S).",
+    "datalog_actions": "can_access(S, O, A) :- Subject(S), Object(O), has_role(S, 'admin'), (A = 'read'; A = 'write')."
 }</t>
         </is>
       </c>
@@ -1282,11 +1143,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.14.0.4"&gt;
-                &lt;Target/&gt;
-                &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.14.0.4.3"&gt;
-                    &lt;Target/&gt;
-                    &lt;Policy PolicyId="RPSlist.14.0.4.3.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.14.0.4.3.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                         &lt;Target&gt;
                             &lt;Subjects&gt;
 &lt;Subject&gt;
@@ -1330,10 +1187,10 @@
       <c r="C15" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "User(U), Role(U, R), MeetingStatus(U, S).",
-    "datalog_objects": "Resource(Res).",
-    "datalog_relationships": "",
-    "datalog_actions": "can_access(U, Res, read) :- User(U), Resource(Res), Role(U, admin), MeetingStatus(U, false)."
+    "datalog_subjects": "Admin(S).",
+    "datalog_objects": "Resource(R).",
+    "datalog_relationships": "has_role(S, \"admin\") :- Admin(S).\nnot_in_meeting(S) :- Admin(S).",
+    "datalog_actions": "can_read(S, R) :- Admin(S), Resource(R), has_role(S, \"admin\"), not_in_meeting(S)."
 }</t>
         </is>
       </c>
@@ -1341,20 +1198,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.15"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;ismeetingflag_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.15.0"&gt;
-            &lt;Target/&gt;
-            &lt;Policy PolicyId="RPSlist.15.0.4" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.15.0.4" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                 &lt;Target/&gt;
                 &lt;Rule Effect="Deny" RuleId="RPSlist.15.0.4.r.1"&gt;
                     &lt;Target/&gt;
@@ -1377,10 +1221,10 @@
       <c r="C16" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S).",
-    "datalog_objects": "Resource(R).",
-    "datalog_relationships": "is_meeting_flag(R) :- Resource(R), R = \"ismeetingflag_rc\".",
-    "datalog_actions": "deny_access(S, R) :- Subject(S), Resource(R), is_meeting_flag(R)."
+    "datalog_subjects": "",
+    "datalog_objects": "",
+    "datalog_relationships": "",
+    "datalog_actions": "deny_all :- false."
 }</t>
         </is>
       </c>
@@ -1388,22 +1232,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.17"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;ismeetingflag_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.17.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.17.0.1"&gt;
-                &lt;Target/&gt;
-                &lt;Policy PolicyId="RPSlist.17.0.1.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.17.0.1.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                     &lt;Target&gt;
                         &lt;Subjects&gt;
                             &lt;Subject&gt;
@@ -1449,10 +1278,10 @@
       <c r="C17" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S).",
-    "datalog_objects": "Resource(R).",
-    "datalog_relationships": "has_role(S, 'admin') :- Subject(S).",
-    "datalog_actions": "can_access(S, R, 'read') :- Subject(S), Resource(R), has_role(S, 'admin'), resource_id(R, 'ismeetingflag_rc')."
+    "datalog_subjects": "Subject(S), role(S, admin).",
+    "datalog_objects": "",
+    "datalog_relationships": "",
+    "datalog_actions": "can_access(S, read) :- Subject(S), role(S, admin)."
 }</t>
         </is>
       </c>
@@ -1460,11 +1289,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.17.0.1.5"&gt;
-                    &lt;Target/&gt;
-                    &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.17.0.1.5.3"&gt;
-                        &lt;Target/&gt;
-                        &lt;Policy PolicyId="RPSlist.17.0.1.5.3.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.17.0.1.5.3.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                             &lt;Target&gt;
 &lt;Subjects&gt;
     &lt;Subject&gt;
@@ -1507,7 +1332,7 @@
     "datalog_subjects": "Subject(S).",
     "datalog_objects": "",
     "datalog_relationships": "",
-    "datalog_actions": "can_access(S, \"read\") :- Subject(S), not role(S, \"false\")."
+    "datalog_actions": "can_read(S) :- Subject(S), not has_role(S)."
 }</t>
         </is>
       </c>
@@ -1515,26 +1340,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.18"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;ismeetingflag_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.18.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.18.0.2"&gt;
-                &lt;Target/&gt;
-                &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.18.0.2.5"&gt;
-                    &lt;Target/&gt;
-                    &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.18.0.2.5.3"&gt;
-                        &lt;Target/&gt;
-                        &lt;Policy PolicyId="RPSlist.18.0.2.5.3.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.18.0.2.5.3.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                             &lt;Target&gt;
 &lt;Subjects&gt;
     &lt;Subject&gt;
@@ -1581,9 +1387,9 @@
         <is>
           <t>{
     "datalog_subjects": "Subject(S).",
-    "datalog_objects": "Resource(R).",
+    "datalog_objects": "",
     "datalog_relationships": "has_role(S, 'admin') :- Subject(S).",
-    "datalog_actions": "can_access(S, R, 'read') :- Subject(S), Resource(R), has_role(S, 'admin'), resource_id(R, 'ismeetingflag_rc').\ncan_access(S, R, 'write') :- Subject(S), Resource(R), has_role(S, 'admin'), resource_id(R, 'ismeetingflag_rc')."
+    "datalog_actions": "can_access(S, 'read') :- Subject(S), has_role(S, 'admin'). can_access(S, 'write') :- Subject(S), has_role(S, 'admin')."
 }</t>
         </is>
       </c>
@@ -1591,28 +1397,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.19"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;paper_review_content_rating_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.19.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.19.0.1"&gt;
-                &lt;Target/&gt;
-                &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.19.0.1.1"&gt;
-                    &lt;Target/&gt;
-                    &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.19.0.1.1.5"&gt;
-                        &lt;Target/&gt;
-                        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.19.0.1.1.5.3"&gt;
-                            &lt;Target/&gt;
-                            &lt;Policy PolicyId="RPSlist.19.0.1.1.5.3.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.19.0.1.1.5.3.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
 &lt;Target&gt;
     &lt;Subjects&gt;
         &lt;Subject&gt;
@@ -1658,10 +1443,10 @@
       <c r="C20" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S).",
-    "datalog_objects": "Resource(R).",
-    "datalog_relationships": "has_role(S, 'admin') :- Subject(S).",
-    "datalog_actions": "can_access(S, R, 'read') :- Subject(S), Resource(R), has_role(S, 'admin'), resource_id(R, 'paper_review_content_rating_rc'). can_access(S, R, 'write') :- Subject(S), Resource(R), has_role(S, 'admin'), resource_id(R, 'paper_review_content_rating_rc')."
+    "datalog_subjects": "Subject(S), has_role(S, 'admin').",
+    "datalog_objects": "Object(O).",
+    "datalog_relationships": "",
+    "datalog_actions": "can_access(S, O, 'read') :- Subject(S), Object(O), has_role(S, 'admin').\ncan_access(S, O, 'write') :- Subject(S), Object(O), has_role(S, 'admin')."
 }</t>
         </is>
       </c>
@@ -1695,7 +1480,7 @@
     "datalog_subjects": "",
     "datalog_objects": "",
     "datalog_relationships": "",
-    "datalog_actions": "deny_all :- false."
+    "datalog_actions": ""
 }</t>
         </is>
       </c>
@@ -1703,24 +1488,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.20"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;paper-review-content-rating_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.20.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.20.0.0"&gt;
-                &lt;Target/&gt;
-                &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.20.0.0.2"&gt;
-                    &lt;Target/&gt;
-                    &lt;Policy PolicyId="RPSlist.20.0.0.2.3" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.20.0.0.2.3" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                         &lt;Target&gt;
                             &lt;Subjects&gt;
 &lt;Subject&gt;
@@ -1753,9 +1521,9 @@
         <is>
           <t>{
     "datalog_subjects": "Subject(S).",
-    "datalog_objects": "Resource(R).",
+    "datalog_objects": "",
     "datalog_relationships": "is_conflicted(S) :- Subject(S).",
-    "datalog_actions": "can_access(S, R) :- Subject(S), Resource(R), not is_conflicted(S)."
+    "datalog_actions": "can_access(S, O, A) :- Subject(S), Object(O), Action(A), not is_conflicted(S)."
 }</t>
         </is>
       </c>
@@ -1816,10 +1584,10 @@
       <c r="C23" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S).",
-    "datalog_objects": "Resource(R).",
-    "datalog_relationships": "has_role(S, \"admin\") :- Subject(S).\nnot_conflicted(S) :- Subject(S).\nhas_resource_attribute(R, \"ismeetingflag_rc\") :- Resource(R).",
-    "datalog_actions": "can_access(S, R, \"read\") :- Subject(S), Resource(R), has_role(S, \"admin\"), not_conflicted(S), has_resource_attribute(R, \"ismeetingflag_rc\")."
+    "datalog_subjects": "Subject(S), role(S, R), isConflicted(S, C).",
+    "datalog_objects": "Resource(Res), isSeeUnassignedAllowed(Res, Flag).",
+    "datalog_relationships": "",
+    "datalog_actions": "can_access(S, Res, read) :- Subject(S), Resource(Res), role(S, \"admin\"), isConflicted(S, \"false\"), isSeeUnassignedAllowed(Res, \"ismeetingflag_rc\")."
 }</t>
         </is>
       </c>
@@ -1827,22 +1595,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.21"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;ismeetingflag_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.21.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.21.0.0"&gt;
-                &lt;Target/&gt;
-                &lt;Policy PolicyId="RPSlist.21.0.0.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.21.0.0.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                     &lt;Target&gt;
                         &lt;Subjects&gt;
                             &lt;Subject&gt;
@@ -1886,10 +1639,10 @@
       <c r="C24" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S).",
+    "datalog_subjects": "Admin(S).",
     "datalog_objects": "Resource(R).",
-    "datalog_relationships": "has_role(S, 'admin') :- Subject(S).\nhas_isEq_subjUserId_resUserId(S, 'false') :- Subject(S).\nhas_resource_id(R, 'ismeetingflag_rc') :- Resource(R).",
-    "datalog_actions": "can_access(S, R, 'read') :- Subject(S), Resource(R), has_role(S, 'admin'), has_isEq_subjUserId_resUserId(S, 'false'), has_resource_id(R, 'ismeetingflag_rc')."
+    "datalog_relationships": "",
+    "datalog_actions": "can_read(S, R) :- Admin(S), Resource(R), role(S, \"admin\"), isEq_subjUserId_resUserId(S, \"false\")."
 }</t>
         </is>
       </c>
@@ -1897,13 +1650,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.21.0.0.2"&gt;
-                    &lt;Target/&gt;
-                    &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.21.0.0.2.5"&gt;
-                        &lt;Target/&gt;
-                        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.21.0.0.2.5.3"&gt;
-                            &lt;Target/&gt;
-                            &lt;Policy PolicyId="RPSlist.21.0.0.2.5.3.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.21.0.0.2.5.3.2" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
 &lt;Target&gt;
     &lt;Subjects&gt;
         &lt;Subject&gt;
@@ -1949,8 +1696,8 @@
           <t>{
     "datalog_subjects": "Subject(S).",
     "datalog_objects": "Object(O).",
-    "datalog_relationships": "has_role(S, admin) :- Subject(S).\nhas_isMeeting(S, false) :- Subject(S).",
-    "datalog_actions": "can_access(S, O, read) :- Subject(S), Object(O), has_role(S, admin), has_isMeeting(S, false)."
+    "datalog_relationships": "has_role(S, \"admin\") :- Subject(S).\nhas_isMeeting(S, \"false\") :- Subject(S).",
+    "datalog_actions": "can_access(S, O, \"read\") :- Subject(S), Object(O), has_role(S, \"admin\"), has_isMeeting(S, \"false\")."
 }</t>
         </is>
       </c>
@@ -1984,7 +1731,7 @@
     "datalog_subjects": "",
     "datalog_objects": "",
     "datalog_relationships": "",
-    "datalog_actions": "deny_all :- false."
+    "datalog_actions": "deny_action(S, O, A) :- Subject(S), Object(O), Action(A)."
 }</t>
         </is>
       </c>
@@ -1992,24 +1739,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.22"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;paper_review_content_rating_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.22.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.22.0.0"&gt;
-                &lt;Target/&gt;
-                &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.22.0.0.2"&gt;
-                    &lt;Target/&gt;
-                    &lt;Policy PolicyId="RPSlist.22.0.0.2.4" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.22.0.0.2.4" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                         &lt;Target&gt;
                             &lt;Subjects&gt;
 &lt;Subject&gt;
@@ -2066,10 +1796,10 @@
       <c r="C27" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S), Admin(A).",
-    "datalog_objects": "Paper(P).",
-    "datalog_relationships": "is_conflicted(S) :- Subject(S).\nsubj_reviews_this_res_paper(S, P) :- Subject(S), Paper(P).\nhas_submitted_review_for_res_paper(S, P) :- Subject(S), Paper(P).",
-    "datalog_actions": "can_read(S, P) :- Subject(S), Paper(P), not is_conflicted(S), subj_reviews_this_res_paper(S, P), not has_submitted_review_for_res_paper(S, P)."
+    "datalog_subjects": "Subject(S).",
+    "datalog_objects": "Resource(R).",
+    "datalog_relationships": "role(S, 'false') :- Subject(S).\nisConflicted(S, 'false') :- Subject(S).\nsubjReviewsThisResPaper(S, 'admin') :- Subject(S).\nhasSubmittedReviewForResPaper(S, 'false') :- Subject(S).",
+    "datalog_actions": "can_read(S, R) :- Subject(S), Resource(R), role(S, 'false'), isConflicted(S, 'false'), subjReviewsThisResPaper(S, 'admin'), hasSubmittedReviewForResPaper(S, 'false')."
 }</t>
         </is>
       </c>
@@ -2077,22 +1807,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.23"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;paper_review_content_rating_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.23.0"&gt;
-            &lt;Target/&gt;
-            &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.23.0.0"&gt;
-                &lt;Target/&gt;
-                &lt;Policy PolicyId="RPSlist.23.0.0.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.23.0.0.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                     &lt;Target&gt;
                         &lt;Subjects&gt;
                             &lt;Subject&gt;
@@ -2124,10 +1839,10 @@
       <c r="C28" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Subject(S).",
+    "datalog_subjects": "Admin(S) :- Subject(S), role(S, \"admin\").",
     "datalog_objects": "Resource(R).",
-    "datalog_relationships": "has_role(S, \"admin\") :- Subject(S).",
-    "datalog_actions": "can_access(S, R) :- Subject(S), Resource(R), has_role(S, \"admin\")."
+    "datalog_relationships": "",
+    "datalog_actions": "can_access(S, R) :- Admin(S), Resource(R)."
 }</t>
         </is>
       </c>
@@ -2135,9 +1850,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.23.0.0.1"&gt;
-                    &lt;Target/&gt;
-                    &lt;Policy PolicyId="RPSlist.23.0.0.1.3" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.23.0.0.1.3" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                         &lt;Target&gt;
                             &lt;Subjects&gt;
 &lt;Subject&gt;
@@ -2169,10 +1882,10 @@
       <c r="C29" t="inlineStr">
         <is>
           <t>{
-    "datalog_subjects": "Admin(S).",
+    "datalog_subjects": "Admin(A).",
     "datalog_objects": "",
-    "datalog_relationships": "",
-    "datalog_actions": "deny_access(S) :- Admin(S), is_conflicted(S)."
+    "datalog_relationships": "is_conflicted(A) :- Admin(A).",
+    "datalog_actions": "can_access(A, O) :- Admin(A), Object(O), not is_conflicted(A)."
 }</t>
         </is>
       </c>
@@ -2180,9 +1893,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.23.0.0.1.5"&gt;
-                        &lt;Target/&gt;
-                        &lt;Policy PolicyId="RPSlist.23.0.0.1.5.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.23.0.0.1.5.1" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                             &lt;Target&gt;
 &lt;Subjects&gt;
     &lt;Subject&gt;
@@ -2232,8 +1943,8 @@
           <t>{
     "datalog_subjects": "Subject(S).",
     "datalog_objects": "Resource(R).",
-    "datalog_relationships": "",
-    "datalog_actions": "can_access(S, R, read) :- Subject(S), Resource(R), role(S, admin), isEq_meetingPaper_resId(R, ismeetingflag_rc)."
+    "datalog_relationships": "has_role(S, \"admin\") :- Subject(S).\nis_meeting_paper_resource(R) :- Resource(R).",
+    "datalog_actions": "can_read(S, R) :- Subject(S), Resource(R), has_role(S, \"admin\"), is_meeting_paper_resource(R)."
 }</t>
         </is>
       </c>
@@ -2241,20 +1952,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>&lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.24"&gt;
-        &lt;Target&gt;
-            &lt;Resources&gt;
-                &lt;Resource&gt;
-                    &lt;ResourceMatch MatchId="urn:oasis:names:tc:xacml:1.0:function:string-equal"&gt;
-                        &lt;AttributeValue DataType="http://www.w3.org/2001/XMLSchema#string"&gt;isMeetingFlag_rc&lt;/AttributeValue&gt;
-                        &lt;ResourceAttributeDesignator AttributeId="urn:oasis:names:tc:xacml:1.0:resource:resource-id" DataType="http://www.w3.org/2001/XMLSchema#string"/&gt;
-                    &lt;/ResourceMatch&gt;
-                &lt;/Resource&gt;
-            &lt;/Resources&gt;
-        &lt;/Target&gt;
-        &lt;PolicySet PolicyCombiningAlgId="urn:oasis:names:tc:xacml:1.0:policy-combining-algorithm:first-applicable" PolicySetId="RPSlist.24.0"&gt;
-            &lt;Target/&gt;
-            &lt;Policy PolicyId="RPSlist.24.0.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
+          <t>&lt;Policy PolicyId="RPSlist.24.0.0" RuleCombiningAlgId="urn:oasis:names:tc:xacml:1.0:rule-combining-algorithm:first-applicable"&gt;
                 &lt;Target&gt;
                     &lt;Subjects&gt;
                         &lt;Subject&gt;
@@ -2301,9 +1999,9 @@
         <is>
           <t>{
     "datalog_subjects": "Subject(S).",
-    "datalog_objects": "Resource(R).",
-    "datalog_relationships": "",
-    "datalog_actions": "can_access(S, R, read) :- Subject(S), Resource(R), role(S, false). can_access(S, R, write) :- Subject(S), Resource(R), role(S, false)."
+    "datalog_objects": "Object(O).",
+    "datalog_relationships": "has_role(S, R) :- Subject(S), Role(R).",
+    "datalog_actions": "can_access(S, O, read) :- Subject(S), Object(O), not has_role(S, \"false\").\ncan_access(S, O, write) :- Subject(S), Object(O), not has_role(S, \"false\")."
 }</t>
         </is>
       </c>

</xml_diff>